<commit_message>
chore: update data of xlsx file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,11 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>"AY bb HJK"</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,17 +603,6 @@
         <v>2.0430882352941175</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D13">
-        <f>SUM(A1:A5) + MAX(B1, AVERAGE(C1:C3, D1))</f>
-        <v>77</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>